<commit_message>
Add extract from free text column
</commit_message>
<xml_diff>
--- a/guidelines/eDischarge-Summary-v2.1-1st-Feb-21.xlsx
+++ b/guidelines/eDischarge-Summary-v2.1-1st-Feb-21.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10811"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42FFACC3-6F6A-4A44-8335-2952440BB05F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{770304EC-493E-C34B-B142-DC04D7D9106C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1297,7 +1297,7 @@
     <t>N</t>
   </si>
   <si>
-    <t>Already in database</t>
+    <t>Extract from Free Text</t>
   </si>
 </sst>
 </file>
@@ -1416,7 +1416,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1433,14 +1433,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1785,7 +1788,7 @@
   <dimension ref="A1:F224"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1793,28 +1796,28 @@
     <col min="1" max="2" width="30" customWidth="1"/>
     <col min="3" max="4" width="12.5" customWidth="1"/>
     <col min="5" max="5" width="37.5" customWidth="1"/>
-    <col min="6" max="6" width="19" customWidth="1"/>
+    <col min="6" max="6" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
     </row>
     <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-    </row>
-    <row r="4" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+    </row>
+    <row r="4" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
@@ -1847,11 +1850,11 @@
       <c r="D5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="9" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="F5" s="7" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>11</v>
       </c>
@@ -1887,8 +1890,8 @@
       <c r="E7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="8" t="s">
-        <v>404</v>
+      <c r="F7" s="6" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="64" x14ac:dyDescent="0.2">
@@ -1907,8 +1910,8 @@
       <c r="E8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="8" t="s">
-        <v>404</v>
+      <c r="F8" s="6" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="96" x14ac:dyDescent="0.2">
@@ -1927,8 +1930,8 @@
       <c r="E9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="8" t="s">
-        <v>404</v>
+      <c r="F9" s="6" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="96" x14ac:dyDescent="0.2">
@@ -1947,8 +1950,8 @@
       <c r="E10" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F10" s="8" t="s">
-        <v>404</v>
+      <c r="F10" s="6" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="64" x14ac:dyDescent="0.2">
@@ -1967,8 +1970,8 @@
       <c r="E11" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="8" t="s">
-        <v>404</v>
+      <c r="F11" s="6" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="64" x14ac:dyDescent="0.2">
@@ -1987,8 +1990,8 @@
       <c r="E12" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F12" s="8" t="s">
-        <v>404</v>
+      <c r="F12" s="6" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="64" x14ac:dyDescent="0.2">
@@ -2007,8 +2010,8 @@
       <c r="E13" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="F13" s="8" t="s">
-        <v>404</v>
+      <c r="F13" s="6" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="64" x14ac:dyDescent="0.2">
@@ -2027,8 +2030,8 @@
       <c r="E14" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="F14" s="8" t="s">
-        <v>404</v>
+      <c r="F14" s="6" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="176" x14ac:dyDescent="0.2">
@@ -2047,8 +2050,8 @@
       <c r="E15" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F15" s="8" t="s">
-        <v>404</v>
+      <c r="F15" s="6" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="208" x14ac:dyDescent="0.2">
@@ -2067,11 +2070,11 @@
       <c r="E16" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="F16" s="8" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="F16" s="6" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>2</v>
       </c>
@@ -2104,11 +2107,11 @@
       <c r="D19" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F19" s="8" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="F19" s="6" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
         <v>11</v>
       </c>
@@ -2144,8 +2147,8 @@
       <c r="E21" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="F21" s="8" t="s">
-        <v>404</v>
+      <c r="F21" s="6" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="64" x14ac:dyDescent="0.2">
@@ -2164,8 +2167,8 @@
       <c r="E22" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="F22" s="8" t="s">
-        <v>404</v>
+      <c r="F22" s="6" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="272" x14ac:dyDescent="0.2">
@@ -2184,8 +2187,8 @@
       <c r="E23" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F23" s="8" t="s">
-        <v>404</v>
+      <c r="F23" s="6" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="64" x14ac:dyDescent="0.2">
@@ -2204,11 +2207,11 @@
       <c r="E24" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="F24" s="8" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="F24" s="6" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>2</v>
       </c>
@@ -2238,11 +2241,11 @@
       <c r="D27" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F27" s="8" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="F27" s="6" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
         <v>11</v>
       </c>
@@ -2278,14 +2281,14 @@
       <c r="E29" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="F29" s="8" t="s">
-        <v>404</v>
+      <c r="F29" s="6" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="4"/>
     </row>
-    <row r="31" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>2</v>
       </c>
@@ -2316,10 +2319,10 @@
         <v>38</v>
       </c>
       <c r="F32" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>11</v>
       </c>
@@ -2355,8 +2358,8 @@
       <c r="E34" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="F34" s="8" t="s">
-        <v>405</v>
+      <c r="F34" s="6" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="160" x14ac:dyDescent="0.2">
@@ -2375,8 +2378,8 @@
       <c r="E35" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="F35" s="8" t="s">
-        <v>405</v>
+      <c r="F35" s="6" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="64" x14ac:dyDescent="0.2">
@@ -2395,11 +2398,11 @@
       <c r="E36" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="F36" s="8" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="F36" s="6" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A38" s="5" t="s">
         <v>2</v>
       </c>
@@ -2429,11 +2432,11 @@
       <c r="D39" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F39" s="8" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="F39" s="6" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A40" s="5" t="s">
         <v>11</v>
       </c>
@@ -2469,8 +2472,8 @@
       <c r="E41" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="F41" s="8" t="s">
-        <v>405</v>
+      <c r="F41" s="6" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="320" x14ac:dyDescent="0.2">
@@ -2489,11 +2492,11 @@
       <c r="E42" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="F42" s="8" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="F42" s="6" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A44" s="5" t="s">
         <v>2</v>
       </c>
@@ -2524,10 +2527,10 @@
         <v>38</v>
       </c>
       <c r="F45" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A46" s="5" t="s">
         <v>11</v>
       </c>
@@ -2563,8 +2566,8 @@
       <c r="E47" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="F47" s="8" t="s">
-        <v>405</v>
+      <c r="F47" s="6" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="64" x14ac:dyDescent="0.2">
@@ -2583,11 +2586,11 @@
       <c r="E48" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="F48" s="8" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="F48" s="6" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A50" s="5" t="s">
         <v>2</v>
       </c>
@@ -2618,10 +2621,10 @@
         <v>18</v>
       </c>
       <c r="F51" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A52" s="5" t="s">
         <v>11</v>
       </c>
@@ -2657,8 +2660,8 @@
       <c r="E53" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="F53" s="8" t="s">
-        <v>405</v>
+      <c r="F53" s="6" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -2677,8 +2680,8 @@
       <c r="E54" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="F54" s="8" t="s">
-        <v>404</v>
+      <c r="F54" s="6" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -2697,8 +2700,8 @@
       <c r="E55" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="F55" s="8" t="s">
-        <v>404</v>
+      <c r="F55" s="6" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -2717,11 +2720,11 @@
       <c r="E56" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="F56" s="8" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="F56" s="6" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A58" s="5" t="s">
         <v>2</v>
       </c>
@@ -2751,11 +2754,11 @@
       <c r="D59" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F59" s="8" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="F59" s="6" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A60" s="5" t="s">
         <v>11</v>
       </c>
@@ -2791,8 +2794,8 @@
       <c r="E61" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="F61" s="8" t="s">
-        <v>404</v>
+      <c r="F61" s="6" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="64" x14ac:dyDescent="0.2">
@@ -2811,8 +2814,8 @@
       <c r="E62" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="F62" s="8" t="s">
-        <v>404</v>
+      <c r="F62" s="6" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -2831,8 +2834,8 @@
       <c r="E63" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="F63" s="8" t="s">
-        <v>404</v>
+      <c r="F63" s="6" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -2851,8 +2854,8 @@
       <c r="E64" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="F64" s="8" t="s">
-        <v>404</v>
+      <c r="F64" s="6" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="112" x14ac:dyDescent="0.2">
@@ -2871,8 +2874,8 @@
       <c r="E65" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="F65" s="8" t="s">
-        <v>404</v>
+      <c r="F65" s="6" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -2891,8 +2894,8 @@
       <c r="E66" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="F66" s="8" t="s">
-        <v>404</v>
+      <c r="F66" s="6" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -2911,8 +2914,8 @@
       <c r="E67" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="F67" s="8" t="s">
-        <v>404</v>
+      <c r="F67" s="6" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="96" x14ac:dyDescent="0.2">
@@ -2931,11 +2934,11 @@
       <c r="E68" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="F68" s="8" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="F68" s="6" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A70" s="5" t="s">
         <v>2</v>
       </c>
@@ -2968,11 +2971,11 @@
       <c r="D71" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F71" s="8" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="F71" s="6" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A72" s="5" t="s">
         <v>11</v>
       </c>
@@ -3008,8 +3011,8 @@
       <c r="E73" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="F73" s="8" t="s">
-        <v>405</v>
+      <c r="F73" s="6" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="176" x14ac:dyDescent="0.2">
@@ -3028,8 +3031,8 @@
       <c r="E74" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="F74" s="8" t="s">
-        <v>405</v>
+      <c r="F74" s="6" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="75" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -3048,8 +3051,8 @@
       <c r="E75" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="F75" s="8" t="s">
-        <v>405</v>
+      <c r="F75" s="6" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="76" spans="1:6" ht="64" x14ac:dyDescent="0.2">
@@ -3068,11 +3071,11 @@
       <c r="E76" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="F76" s="8" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="F76" s="6" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A78" s="5" t="s">
         <v>2</v>
       </c>
@@ -3105,11 +3108,11 @@
       <c r="D79" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F79" s="8" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="F79" s="6" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A80" s="5" t="s">
         <v>11</v>
       </c>
@@ -3145,8 +3148,8 @@
       <c r="E81" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="F81" s="8" t="s">
-        <v>405</v>
+      <c r="F81" s="6" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="82" spans="1:6" ht="64" x14ac:dyDescent="0.2">
@@ -3165,8 +3168,8 @@
       <c r="E82" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="F82" s="8" t="s">
-        <v>405</v>
+      <c r="F82" s="6" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="83" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -3185,8 +3188,8 @@
       <c r="E83" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="F83" s="8" t="s">
-        <v>405</v>
+      <c r="F83" s="6" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="84" spans="1:6" ht="64" x14ac:dyDescent="0.2">
@@ -3205,8 +3208,8 @@
       <c r="E84" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="F84" s="8" t="s">
-        <v>405</v>
+      <c r="F84" s="6" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="85" spans="1:6" ht="96" x14ac:dyDescent="0.2">
@@ -3225,8 +3228,8 @@
       <c r="E85" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="F85" s="8" t="s">
-        <v>405</v>
+      <c r="F85" s="6" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="86" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -3245,8 +3248,8 @@
       <c r="E86" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="F86" s="8" t="s">
-        <v>405</v>
+      <c r="F86" s="6" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="87" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -3265,11 +3268,11 @@
       <c r="E87" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="F87" s="8" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="F87" s="6" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A89" s="5" t="s">
         <v>2</v>
       </c>
@@ -3302,11 +3305,11 @@
       <c r="D90" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F90" s="8" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="F90" s="6" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A91" s="5" t="s">
         <v>11</v>
       </c>
@@ -3342,11 +3345,11 @@
       <c r="E92" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="F92" s="8" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="F92" s="6" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A94" s="5" t="s">
         <v>2</v>
       </c>
@@ -3377,10 +3380,10 @@
         <v>38</v>
       </c>
       <c r="F95" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A96" s="5" t="s">
         <v>11</v>
       </c>
@@ -3416,8 +3419,8 @@
       <c r="E97" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="F97" s="8" t="s">
-        <v>405</v>
+      <c r="F97" s="6" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="98" spans="1:6" ht="112" x14ac:dyDescent="0.2">
@@ -3436,16 +3439,16 @@
       <c r="E98" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="F98" s="8" t="s">
-        <v>405</v>
+      <c r="F98" s="6" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F99" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A100" s="5" t="s">
         <v>2</v>
       </c>
@@ -3476,10 +3479,10 @@
         <v>38</v>
       </c>
       <c r="F101" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A102" s="5" t="s">
         <v>11</v>
       </c>
@@ -3515,8 +3518,8 @@
       <c r="E103" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="F103" s="8" t="s">
-        <v>405</v>
+      <c r="F103" s="6" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="104" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -3535,11 +3538,11 @@
       <c r="E104" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="F104" s="8" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="F104" s="6" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A106" s="5" t="s">
         <v>2</v>
       </c>
@@ -3570,10 +3573,10 @@
         <v>18</v>
       </c>
       <c r="F107" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="108" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A108" s="5" t="s">
         <v>11</v>
       </c>
@@ -3609,8 +3612,8 @@
       <c r="E109" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="F109" s="8" t="s">
-        <v>405</v>
+      <c r="F109" s="6" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="110" spans="1:6" ht="112" x14ac:dyDescent="0.2">
@@ -3629,8 +3632,8 @@
       <c r="E110" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="F110" s="8" t="s">
-        <v>405</v>
+      <c r="F110" s="6" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="111" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -3649,8 +3652,8 @@
       <c r="E111" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="F111" s="8" t="s">
-        <v>405</v>
+      <c r="F111" s="6" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="112" spans="1:6" ht="112" x14ac:dyDescent="0.2">
@@ -3669,8 +3672,8 @@
       <c r="E112" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="F112" s="8" t="s">
-        <v>405</v>
+      <c r="F112" s="6" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="113" spans="1:6" ht="224" x14ac:dyDescent="0.2">
@@ -3689,8 +3692,8 @@
       <c r="E113" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="F113" s="8" t="s">
-        <v>405</v>
+      <c r="F113" s="6" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="114" spans="1:6" ht="304" x14ac:dyDescent="0.2">
@@ -3709,8 +3712,8 @@
       <c r="E114" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="F114" s="8" t="s">
-        <v>405</v>
+      <c r="F114" s="6" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="115" spans="1:6" ht="96" x14ac:dyDescent="0.2">
@@ -3729,8 +3732,8 @@
       <c r="E115" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="F115" s="8" t="s">
-        <v>405</v>
+      <c r="F115" s="6" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="116" spans="1:6" ht="64" x14ac:dyDescent="0.2">
@@ -3749,11 +3752,11 @@
       <c r="E116" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="F116" s="8" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="118" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="F116" s="6" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A118" s="5" t="s">
         <v>2</v>
       </c>
@@ -3783,11 +3786,11 @@
       <c r="D119" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F119" s="8" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="120" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="F119" s="6" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A120" s="5" t="s">
         <v>11</v>
       </c>
@@ -3823,8 +3826,8 @@
       <c r="E121" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="F121" s="8" t="s">
-        <v>405</v>
+      <c r="F121" s="6" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="122" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -3843,8 +3846,8 @@
       <c r="E122" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="F122" s="8" t="s">
-        <v>405</v>
+      <c r="F122" s="6" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="123" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -3863,11 +3866,11 @@
       <c r="E123" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="F123" s="8" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="125" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="F123" s="6" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A125" s="5" t="s">
         <v>2</v>
       </c>
@@ -3897,11 +3900,11 @@
       <c r="D126" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F126" s="8" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="127" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="F126" s="6" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A127" s="5" t="s">
         <v>11</v>
       </c>
@@ -3937,8 +3940,8 @@
       <c r="E128" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="F128" s="8" t="s">
-        <v>404</v>
+      <c r="F128" s="6" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="129" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -3962,8 +3965,8 @@
       <c r="E130" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="F130" s="8" t="s">
-        <v>404</v>
+      <c r="F130" s="6" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="131" spans="1:6" ht="96" x14ac:dyDescent="0.2">
@@ -3982,8 +3985,8 @@
       <c r="E131" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="F131" s="8" t="s">
-        <v>404</v>
+      <c r="F131" s="6" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="132" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -4002,8 +4005,8 @@
       <c r="E132" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="F132" s="8" t="s">
-        <v>404</v>
+      <c r="F132" s="6" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="133" spans="1:6" ht="272" x14ac:dyDescent="0.2">
@@ -4022,8 +4025,8 @@
       <c r="E133" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="F133" s="8" t="s">
-        <v>404</v>
+      <c r="F133" s="6" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="134" spans="1:6" ht="96" x14ac:dyDescent="0.2">
@@ -4042,8 +4045,8 @@
       <c r="E134" s="3" t="s">
         <v>231</v>
       </c>
-      <c r="F134" s="8" t="s">
-        <v>404</v>
+      <c r="F134" s="6" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="135" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -4062,8 +4065,8 @@
       <c r="E135" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="F135" s="8" t="s">
-        <v>404</v>
+      <c r="F135" s="6" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="136" spans="1:6" ht="144" x14ac:dyDescent="0.2">
@@ -4082,8 +4085,8 @@
       <c r="E136" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="F136" s="8" t="s">
-        <v>404</v>
+      <c r="F136" s="6" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="137" spans="1:6" ht="240" x14ac:dyDescent="0.2">
@@ -4102,8 +4105,8 @@
       <c r="E137" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="F137" s="8" t="s">
-        <v>404</v>
+      <c r="F137" s="6" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="138" spans="1:6" ht="240" x14ac:dyDescent="0.2">
@@ -4122,8 +4125,8 @@
       <c r="E138" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="F138" s="8" t="s">
-        <v>404</v>
+      <c r="F138" s="6" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="139" spans="1:6" ht="224" x14ac:dyDescent="0.2">
@@ -4142,8 +4145,8 @@
       <c r="E139" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="F139" s="8" t="s">
-        <v>404</v>
+      <c r="F139" s="6" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="140" spans="1:6" ht="350" x14ac:dyDescent="0.2">
@@ -4162,8 +4165,8 @@
       <c r="E140" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="F140" s="8" t="s">
-        <v>404</v>
+      <c r="F140" s="6" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="141" spans="1:6" ht="320" x14ac:dyDescent="0.2">
@@ -4182,8 +4185,8 @@
       <c r="E141" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="F141" s="8" t="s">
-        <v>404</v>
+      <c r="F141" s="6" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="142" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
@@ -4202,8 +4205,8 @@
       <c r="E142" s="3" t="s">
         <v>251</v>
       </c>
-      <c r="F142" s="8" t="s">
-        <v>404</v>
+      <c r="F142" s="6" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="143" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
@@ -4222,8 +4225,8 @@
       <c r="E143" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="F143" s="8" t="s">
-        <v>404</v>
+      <c r="F143" s="6" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="144" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -4242,8 +4245,8 @@
       <c r="E144" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="F144" s="8" t="s">
-        <v>404</v>
+      <c r="F144" s="6" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="145" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
@@ -4262,8 +4265,8 @@
       <c r="E145" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="F145" s="8" t="s">
-        <v>404</v>
+      <c r="F145" s="6" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="146" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -4282,8 +4285,8 @@
       <c r="E146" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="F146" s="8" t="s">
-        <v>404</v>
+      <c r="F146" s="6" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="147" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -4302,8 +4305,8 @@
       <c r="E147" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="F147" s="8" t="s">
-        <v>404</v>
+      <c r="F147" s="6" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="148" spans="1:6" ht="365" x14ac:dyDescent="0.2">
@@ -4322,8 +4325,8 @@
       <c r="E148" s="3" t="s">
         <v>267</v>
       </c>
-      <c r="F148" s="8" t="s">
-        <v>404</v>
+      <c r="F148" s="6" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="149" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -4342,8 +4345,8 @@
       <c r="E149" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="F149" s="8" t="s">
-        <v>404</v>
+      <c r="F149" s="6" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="150" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -4362,8 +4365,8 @@
       <c r="E150" s="3" t="s">
         <v>273</v>
       </c>
-      <c r="F150" s="8" t="s">
-        <v>404</v>
+      <c r="F150" s="6" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="151" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -4382,8 +4385,8 @@
       <c r="E151" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="F151" s="8" t="s">
-        <v>404</v>
+      <c r="F151" s="6" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="152" spans="1:6" ht="208" x14ac:dyDescent="0.2">
@@ -4402,8 +4405,8 @@
       <c r="E152" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="F152" s="8" t="s">
-        <v>404</v>
+      <c r="F152" s="6" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="153" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -4422,8 +4425,8 @@
       <c r="E153" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="F153" s="8" t="s">
-        <v>404</v>
+      <c r="F153" s="6" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="154" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -4442,8 +4445,8 @@
       <c r="E154" s="3" t="s">
         <v>283</v>
       </c>
-      <c r="F154" s="8" t="s">
-        <v>404</v>
+      <c r="F154" s="6" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="155" spans="1:6" ht="64" x14ac:dyDescent="0.2">
@@ -4462,8 +4465,8 @@
       <c r="E155" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="F155" s="8" t="s">
-        <v>404</v>
+      <c r="F155" s="6" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="156" spans="1:6" ht="96" x14ac:dyDescent="0.2">
@@ -4482,8 +4485,8 @@
       <c r="E156" s="3" t="s">
         <v>288</v>
       </c>
-      <c r="F156" s="8" t="s">
-        <v>404</v>
+      <c r="F156" s="6" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="157" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -4502,8 +4505,8 @@
       <c r="E157" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="F157" s="8" t="s">
-        <v>404</v>
+      <c r="F157" s="6" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="158" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -4522,8 +4525,8 @@
       <c r="E158" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="F158" s="8" t="s">
-        <v>404</v>
+      <c r="F158" s="6" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="159" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
@@ -4542,8 +4545,8 @@
       <c r="E159" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="F159" s="8" t="s">
-        <v>404</v>
+      <c r="F159" s="6" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="160" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -4562,8 +4565,8 @@
       <c r="E160" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="F160" s="8" t="s">
-        <v>404</v>
+      <c r="F160" s="6" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="161" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -4582,8 +4585,8 @@
       <c r="E161" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="F161" s="8" t="s">
-        <v>404</v>
+      <c r="F161" s="6" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="162" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -4602,8 +4605,8 @@
       <c r="E162" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="F162" s="8" t="s">
-        <v>404</v>
+      <c r="F162" s="6" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="163" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -4622,8 +4625,8 @@
       <c r="E163" s="3" t="s">
         <v>283</v>
       </c>
-      <c r="F163" s="8" t="s">
-        <v>404</v>
+      <c r="F163" s="6" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="164" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -4642,8 +4645,8 @@
       <c r="E164" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="F164" s="8" t="s">
-        <v>404</v>
+      <c r="F164" s="6" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="165" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -4662,11 +4665,14 @@
       <c r="E165" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="F165" s="8" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="167" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="F165" s="6" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F166" s="6"/>
+    </row>
+    <row r="167" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A167" s="5" t="s">
         <v>2</v>
       </c>
@@ -4699,11 +4705,11 @@
       <c r="D168" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F168" s="8" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="169" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="F168" s="6" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A169" s="5" t="s">
         <v>11</v>
       </c>
@@ -4739,8 +4745,8 @@
       <c r="E170" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="F170" s="8" t="s">
-        <v>405</v>
+      <c r="F170" s="6" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="171" spans="1:6" ht="176" x14ac:dyDescent="0.2">
@@ -4759,8 +4765,8 @@
       <c r="E171" s="3" t="s">
         <v>309</v>
       </c>
-      <c r="F171" s="8" t="s">
-        <v>405</v>
+      <c r="F171" s="6" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="172" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -4780,7 +4786,7 @@
         <v>49</v>
       </c>
       <c r="F172" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="173" spans="1:6" ht="64" x14ac:dyDescent="0.2">
@@ -4799,8 +4805,8 @@
       <c r="E173" s="3" t="s">
         <v>313</v>
       </c>
-      <c r="F173" s="8" t="s">
-        <v>405</v>
+      <c r="F173" s="6" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="174" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -4819,8 +4825,8 @@
       <c r="E174" s="3" t="s">
         <v>316</v>
       </c>
-      <c r="F174" s="8" t="s">
-        <v>405</v>
+      <c r="F174" s="6" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="175" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
@@ -4839,8 +4845,8 @@
       <c r="E175" s="3" t="s">
         <v>319</v>
       </c>
-      <c r="F175" s="8" t="s">
-        <v>405</v>
+      <c r="F175" s="6" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="176" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
@@ -4859,8 +4865,8 @@
       <c r="E176" s="3" t="s">
         <v>322</v>
       </c>
-      <c r="F176" s="8" t="s">
-        <v>405</v>
+      <c r="F176" s="6" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="177" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -4879,8 +4885,8 @@
       <c r="E177" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="F177" s="8" t="s">
-        <v>405</v>
+      <c r="F177" s="6" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="178" spans="1:6" ht="208" x14ac:dyDescent="0.2">
@@ -4899,8 +4905,8 @@
       <c r="E178" s="3" t="s">
         <v>326</v>
       </c>
-      <c r="F178" s="8" t="s">
-        <v>405</v>
+      <c r="F178" s="6" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="179" spans="1:6" ht="64" x14ac:dyDescent="0.2">
@@ -4919,8 +4925,8 @@
       <c r="E179" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="F179" s="8" t="s">
-        <v>405</v>
+      <c r="F179" s="6" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="180" spans="1:6" ht="64" x14ac:dyDescent="0.2">
@@ -4939,11 +4945,11 @@
       <c r="E180" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="F180" s="8" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="182" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="F180" s="6" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A182" s="5" t="s">
         <v>2</v>
       </c>
@@ -4973,11 +4979,11 @@
       <c r="D183" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F183" s="8" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="184" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="F183" s="6" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A184" s="5" t="s">
         <v>11</v>
       </c>
@@ -5013,8 +5019,8 @@
       <c r="E185" s="3" t="s">
         <v>334</v>
       </c>
-      <c r="F185" s="8" t="s">
-        <v>405</v>
+      <c r="F185" s="6" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="186" spans="1:6" ht="144" x14ac:dyDescent="0.2">
@@ -5033,11 +5039,14 @@
       <c r="E186" s="3" t="s">
         <v>337</v>
       </c>
-      <c r="F186" s="8" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="188" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="F186" s="6" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F187" s="10"/>
+    </row>
+    <row r="188" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A188" s="5" t="s">
         <v>2</v>
       </c>
@@ -5068,10 +5077,10 @@
         <v>18</v>
       </c>
       <c r="F189" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="190" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A190" s="5" t="s">
         <v>11</v>
       </c>
@@ -5107,11 +5116,11 @@
       <c r="E191" s="3" t="s">
         <v>341</v>
       </c>
-      <c r="F191" s="8" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="193" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="F191" s="6" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A193" s="5" t="s">
         <v>2</v>
       </c>
@@ -5142,10 +5151,10 @@
         <v>18</v>
       </c>
       <c r="F194" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="195" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A195" s="5" t="s">
         <v>11</v>
       </c>
@@ -5181,8 +5190,8 @@
       <c r="E196" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="F196" s="8" t="s">
-        <v>405</v>
+      <c r="F196" s="6" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="197" spans="1:6" ht="112" x14ac:dyDescent="0.2">
@@ -5201,8 +5210,8 @@
       <c r="E197" s="3" t="s">
         <v>347</v>
       </c>
-      <c r="F197" s="8" t="s">
-        <v>405</v>
+      <c r="F197" s="6" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="198" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -5221,8 +5230,8 @@
       <c r="E198" s="3" t="s">
         <v>350</v>
       </c>
-      <c r="F198" s="8" t="s">
-        <v>405</v>
+      <c r="F198" s="6" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="199" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -5241,8 +5250,8 @@
       <c r="E199" s="3" t="s">
         <v>353</v>
       </c>
-      <c r="F199" s="8" t="s">
-        <v>405</v>
+      <c r="F199" s="6" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="200" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -5261,8 +5270,8 @@
       <c r="E200" s="3" t="s">
         <v>356</v>
       </c>
-      <c r="F200" s="8" t="s">
-        <v>405</v>
+      <c r="F200" s="6" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="201" spans="1:6" ht="64" x14ac:dyDescent="0.2">
@@ -5281,11 +5290,11 @@
       <c r="E201" s="3" t="s">
         <v>359</v>
       </c>
-      <c r="F201" s="8" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="203" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="F201" s="6" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="203" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A203" s="5" t="s">
         <v>2</v>
       </c>
@@ -5318,11 +5327,11 @@
       <c r="D204" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F204" s="8" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="205" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="F204" s="6" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="205" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A205" s="5" t="s">
         <v>11</v>
       </c>
@@ -5358,8 +5367,8 @@
       <c r="E206" s="3" t="s">
         <v>364</v>
       </c>
-      <c r="F206" s="8" t="s">
-        <v>404</v>
+      <c r="F206" s="6" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="207" spans="1:6" ht="64" x14ac:dyDescent="0.2">
@@ -5378,8 +5387,8 @@
       <c r="E207" s="3" t="s">
         <v>367</v>
       </c>
-      <c r="F207" s="8" t="s">
-        <v>404</v>
+      <c r="F207" s="6" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="208" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -5398,8 +5407,8 @@
       <c r="E208" s="3" t="s">
         <v>370</v>
       </c>
-      <c r="F208" s="8" t="s">
-        <v>404</v>
+      <c r="F208" s="6" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="209" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -5418,8 +5427,8 @@
       <c r="E209" s="3" t="s">
         <v>373</v>
       </c>
-      <c r="F209" s="8" t="s">
-        <v>404</v>
+      <c r="F209" s="6" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="210" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -5438,8 +5447,8 @@
       <c r="E210" s="3" t="s">
         <v>376</v>
       </c>
-      <c r="F210" s="8" t="s">
-        <v>404</v>
+      <c r="F210" s="6" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="211" spans="1:6" ht="64" x14ac:dyDescent="0.2">
@@ -5458,8 +5467,8 @@
       <c r="E211" s="3" t="s">
         <v>379</v>
       </c>
-      <c r="F211" s="8" t="s">
-        <v>404</v>
+      <c r="F211" s="6" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="212" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -5478,8 +5487,8 @@
       <c r="E212" s="3" t="s">
         <v>382</v>
       </c>
-      <c r="F212" s="8" t="s">
-        <v>404</v>
+      <c r="F212" s="6" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="213" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -5498,11 +5507,14 @@
       <c r="E213" s="3" t="s">
         <v>385</v>
       </c>
-      <c r="F213" s="8" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="215" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="F213" s="6" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="214" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F214" s="6"/>
+    </row>
+    <row r="215" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A215" s="5" t="s">
         <v>2</v>
       </c>
@@ -5532,11 +5544,11 @@
       <c r="D216" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F216" s="8" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="217" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="F216" s="6" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="217" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A217" s="5" t="s">
         <v>11</v>
       </c>
@@ -5572,8 +5584,8 @@
       <c r="E218" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="F218" s="8" t="s">
-        <v>404</v>
+      <c r="F218" s="6" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="219" spans="1:6" ht="160" x14ac:dyDescent="0.2">
@@ -5592,8 +5604,8 @@
       <c r="E219" s="3" t="s">
         <v>390</v>
       </c>
-      <c r="F219" s="8" t="s">
-        <v>404</v>
+      <c r="F219" s="6" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="220" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -5612,8 +5624,8 @@
       <c r="E220" s="3" t="s">
         <v>392</v>
       </c>
-      <c r="F220" s="8" t="s">
-        <v>404</v>
+      <c r="F220" s="6" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="221" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -5632,8 +5644,8 @@
       <c r="E221" s="3" t="s">
         <v>394</v>
       </c>
-      <c r="F221" s="8" t="s">
-        <v>404</v>
+      <c r="F221" s="6" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="222" spans="1:6" ht="112" x14ac:dyDescent="0.2">
@@ -5652,8 +5664,8 @@
       <c r="E222" s="3" t="s">
         <v>397</v>
       </c>
-      <c r="F222" s="8" t="s">
-        <v>404</v>
+      <c r="F222" s="6" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="223" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -5672,8 +5684,8 @@
       <c r="E223" s="3" t="s">
         <v>400</v>
       </c>
-      <c r="F223" s="8" t="s">
-        <v>404</v>
+      <c r="F223" s="6" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="224" spans="1:6" ht="64" x14ac:dyDescent="0.2">
@@ -5692,8 +5704,8 @@
       <c r="E224" s="3" t="s">
         <v>403</v>
       </c>
-      <c r="F224" s="8" t="s">
-        <v>404</v>
+      <c r="F224" s="6" t="s">
+        <v>405</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Guidelines to pydantic updates
</commit_message>
<xml_diff>
--- a/guidelines/eDischarge-Summary-v2.1-1st-Feb-21.xlsx
+++ b/guidelines/eDischarge-Summary-v2.1-1st-Feb-21.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/simonellershaw/Documents/discharge-summaries/guidelines/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96FCEC8F-73DF-E447-BE4A-AEBDF9D146DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B347C508-13DE-9E49-98C8-77AE0C22C4AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="945" uniqueCount="408">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="947" uniqueCount="410">
   <si>
     <t>E Discharge</t>
   </si>
@@ -1326,6 +1326,12 @@
   </si>
   <si>
     <t>Follow previous formatting convention</t>
+  </si>
+  <si>
+    <t>A structural representation of the elements carried by the dose syntax in 'Parsable doseStrength / timing' i.e. dose strength, dose timing, dose duration and maximum dose.</t>
+  </si>
+  <si>
+    <t>Description from https://developer.nhs.uk/apis/itk3tocedischarge-2-9-0/explore_medication.html</t>
   </si>
 </sst>
 </file>
@@ -1527,12 +1533,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1546,6 +1546,12 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1855,8 +1861,8 @@
   </sheetPr>
   <dimension ref="A1:G228"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
-      <selection activeCell="G156" sqref="G156"/>
+    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
+      <selection activeCell="G134" sqref="G134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1865,28 +1871,28 @@
     <col min="2" max="2" width="30" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="12.5" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="37.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="74.1640625" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="87" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
     </row>
     <row r="2" spans="1:6" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="15"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="13"/>
     </row>
     <row r="3" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="4" spans="1:6" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1905,7 +1911,7 @@
       <c r="E4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="16" t="s">
+      <c r="F4" s="14" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1923,7 +1929,7 @@
         <v>11</v>
       </c>
       <c r="E5" s="2"/>
-      <c r="F5" s="15"/>
+      <c r="F5" s="13"/>
     </row>
     <row r="6" spans="1:6" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
@@ -1941,7 +1947,7 @@
       <c r="E6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="15"/>
+      <c r="F6" s="13"/>
     </row>
     <row r="7" spans="1:6" s="1" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
@@ -1959,7 +1965,7 @@
       <c r="E7" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="15"/>
+      <c r="F7" s="13"/>
     </row>
     <row r="8" spans="1:6" s="1" customFormat="1" ht="74.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
@@ -1977,7 +1983,7 @@
       <c r="E8" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="15"/>
+      <c r="F8" s="13"/>
     </row>
     <row r="9" spans="1:6" s="1" customFormat="1" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
@@ -1995,7 +2001,7 @@
       <c r="E9" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="F9" s="15"/>
+      <c r="F9" s="13"/>
     </row>
     <row r="10" spans="1:6" s="1" customFormat="1" ht="102" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
@@ -2013,7 +2019,7 @@
       <c r="E10" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="F10" s="15"/>
+      <c r="F10" s="13"/>
     </row>
     <row r="11" spans="1:6" s="1" customFormat="1" ht="74.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
@@ -2031,7 +2037,7 @@
       <c r="E11" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="F11" s="15"/>
+      <c r="F11" s="13"/>
     </row>
     <row r="12" spans="1:6" s="1" customFormat="1" ht="74.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
@@ -2049,7 +2055,7 @@
       <c r="E12" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="F12" s="15"/>
+      <c r="F12" s="13"/>
     </row>
     <row r="13" spans="1:6" s="1" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
@@ -2067,7 +2073,7 @@
       <c r="E13" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="F13" s="15"/>
+      <c r="F13" s="13"/>
     </row>
     <row r="14" spans="1:6" s="1" customFormat="1" ht="74.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
@@ -2085,7 +2091,7 @@
       <c r="E14" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="F14" s="15"/>
+      <c r="F14" s="13"/>
     </row>
     <row r="15" spans="1:6" s="1" customFormat="1" ht="156.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
@@ -2103,7 +2109,7 @@
       <c r="E15" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="F15" s="15"/>
+      <c r="F15" s="13"/>
     </row>
     <row r="16" spans="1:6" s="1" customFormat="1" ht="185.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
@@ -2121,7 +2127,7 @@
       <c r="E16" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="F16" s="15"/>
+      <c r="F16" s="13"/>
     </row>
     <row r="17" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="18" spans="1:6" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2140,7 +2146,7 @@
       <c r="E18" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F18" s="15"/>
+      <c r="F18" s="13"/>
     </row>
     <row r="19" spans="1:6" s="1" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
@@ -2156,7 +2162,7 @@
         <v>11</v>
       </c>
       <c r="E19" s="2"/>
-      <c r="F19" s="15"/>
+      <c r="F19" s="13"/>
     </row>
     <row r="20" spans="1:6" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
@@ -2174,7 +2180,7 @@
       <c r="E20" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F20" s="15"/>
+      <c r="F20" s="13"/>
     </row>
     <row r="21" spans="1:6" s="1" customFormat="1" ht="115.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
@@ -2188,7 +2194,7 @@
       </c>
       <c r="D21" s="6"/>
       <c r="E21" s="7"/>
-      <c r="F21" s="15"/>
+      <c r="F21" s="13"/>
     </row>
     <row r="22" spans="1:6" s="1" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
@@ -2206,7 +2212,7 @@
       <c r="E22" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="F22" s="15"/>
+      <c r="F22" s="13"/>
     </row>
     <row r="23" spans="1:6" s="1" customFormat="1" ht="253.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
@@ -2224,7 +2230,7 @@
       <c r="E23" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="F23" s="15"/>
+      <c r="F23" s="13"/>
     </row>
     <row r="24" spans="1:6" s="1" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
@@ -2242,7 +2248,7 @@
       <c r="E24" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="F24" s="15"/>
+      <c r="F24" s="13"/>
     </row>
     <row r="25" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="26" spans="1:6" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2261,7 +2267,7 @@
       <c r="E26" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F26" s="15"/>
+      <c r="F26" s="13"/>
     </row>
     <row r="27" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
@@ -2275,7 +2281,7 @@
         <v>19</v>
       </c>
       <c r="E27" s="2"/>
-      <c r="F27" s="15"/>
+      <c r="F27" s="13"/>
     </row>
     <row r="28" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
@@ -2293,7 +2299,7 @@
       <c r="E28" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F28" s="15"/>
+      <c r="F28" s="13"/>
     </row>
     <row r="29" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
@@ -2311,7 +2317,7 @@
       <c r="E29" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="F29" s="15"/>
+      <c r="F29" s="13"/>
     </row>
     <row r="30" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="5"/>
@@ -2319,7 +2325,7 @@
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
-      <c r="F30" s="15"/>
+      <c r="F30" s="13"/>
     </row>
     <row r="31" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
@@ -2337,7 +2343,7 @@
       <c r="E31" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F31" s="15"/>
+      <c r="F31" s="13"/>
     </row>
     <row r="32" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
@@ -2351,7 +2357,7 @@
         <v>39</v>
       </c>
       <c r="E32" s="2"/>
-      <c r="F32" s="15"/>
+      <c r="F32" s="13"/>
     </row>
     <row r="33" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
@@ -2369,7 +2375,7 @@
       <c r="E33" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F33" s="15"/>
+      <c r="F33" s="13"/>
     </row>
     <row r="34" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
@@ -2387,7 +2393,7 @@
       <c r="E34" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="F34" s="15"/>
+      <c r="F34" s="13"/>
     </row>
     <row r="35" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
@@ -2405,7 +2411,7 @@
       <c r="E35" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="F35" s="15"/>
+      <c r="F35" s="13"/>
     </row>
     <row r="36" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
@@ -2423,7 +2429,7 @@
       <c r="E36" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="F36" s="15"/>
+      <c r="F36" s="13"/>
     </row>
     <row r="37" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="38" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2442,7 +2448,7 @@
       <c r="E38" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F38" s="15"/>
+      <c r="F38" s="13"/>
     </row>
     <row r="39" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
@@ -2456,7 +2462,7 @@
         <v>19</v>
       </c>
       <c r="E39" s="2"/>
-      <c r="F39" s="15"/>
+      <c r="F39" s="13"/>
     </row>
     <row r="40" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
@@ -2474,7 +2480,7 @@
       <c r="E40" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F40" s="15"/>
+      <c r="F40" s="13"/>
     </row>
     <row r="41" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="8" t="s">
@@ -2488,7 +2494,7 @@
       </c>
       <c r="D41" s="6"/>
       <c r="E41" s="7"/>
-      <c r="F41" s="15"/>
+      <c r="F41" s="13"/>
     </row>
     <row r="42" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="5" t="s">
@@ -2506,7 +2512,7 @@
       <c r="E42" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="F42" s="15"/>
+      <c r="F42" s="13"/>
     </row>
     <row r="43" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="44" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2525,7 +2531,7 @@
       <c r="E44" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F44" s="15"/>
+      <c r="F44" s="13"/>
     </row>
     <row r="45" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
@@ -2539,7 +2545,7 @@
         <v>39</v>
       </c>
       <c r="E45" s="2"/>
-      <c r="F45" s="15"/>
+      <c r="F45" s="13"/>
     </row>
     <row r="46" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
@@ -2557,7 +2563,7 @@
       <c r="E46" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F46" s="15"/>
+      <c r="F46" s="13"/>
     </row>
     <row r="47" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="5" t="s">
@@ -2571,7 +2577,7 @@
       </c>
       <c r="D47" s="6"/>
       <c r="E47" s="7"/>
-      <c r="F47" s="15"/>
+      <c r="F47" s="13"/>
     </row>
     <row r="48" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="5" t="s">
@@ -2589,7 +2595,7 @@
       <c r="E48" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="F48" s="15"/>
+      <c r="F48" s="13"/>
     </row>
     <row r="49" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="50" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2608,7 +2614,7 @@
       <c r="E50" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F50" s="15"/>
+      <c r="F50" s="13"/>
     </row>
     <row r="51" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
@@ -2622,7 +2628,7 @@
         <v>19</v>
       </c>
       <c r="E51" s="2"/>
-      <c r="F51" s="15"/>
+      <c r="F51" s="13"/>
     </row>
     <row r="52" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
@@ -2640,7 +2646,7 @@
       <c r="E52" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F52" s="15"/>
+      <c r="F52" s="13"/>
     </row>
     <row r="53" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="5" t="s">
@@ -2658,7 +2664,7 @@
       <c r="E53" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="F53" s="15"/>
+      <c r="F53" s="13"/>
     </row>
     <row r="54" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="5" t="s">
@@ -2676,7 +2682,7 @@
       <c r="E54" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="F54" s="15"/>
+      <c r="F54" s="13"/>
     </row>
     <row r="55" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="5" t="s">
@@ -2694,7 +2700,7 @@
       <c r="E55" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="F55" s="15"/>
+      <c r="F55" s="13"/>
     </row>
     <row r="56" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="5" t="s">
@@ -2712,7 +2718,7 @@
       <c r="E56" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="F56" s="15"/>
+      <c r="F56" s="13"/>
     </row>
     <row r="57" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="58" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2731,7 +2737,7 @@
       <c r="E58" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F58" s="15"/>
+      <c r="F58" s="13"/>
     </row>
     <row r="59" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
@@ -2745,7 +2751,7 @@
         <v>19</v>
       </c>
       <c r="E59" s="2"/>
-      <c r="F59" s="15"/>
+      <c r="F59" s="13"/>
     </row>
     <row r="60" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
@@ -2763,7 +2769,7 @@
       <c r="E60" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F60" s="15"/>
+      <c r="F60" s="13"/>
     </row>
     <row r="61" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="5" t="s">
@@ -2781,7 +2787,7 @@
       <c r="E61" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="F61" s="15"/>
+      <c r="F61" s="13"/>
     </row>
     <row r="62" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="5" t="s">
@@ -2799,7 +2805,7 @@
       <c r="E62" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="F62" s="15"/>
+      <c r="F62" s="13"/>
     </row>
     <row r="63" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="5" t="s">
@@ -2817,7 +2823,7 @@
       <c r="E63" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="F63" s="15"/>
+      <c r="F63" s="13"/>
     </row>
     <row r="64" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="5" t="s">
@@ -2835,7 +2841,7 @@
       <c r="E64" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="F64" s="15"/>
+      <c r="F64" s="13"/>
     </row>
     <row r="65" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="5" t="s">
@@ -2853,7 +2859,7 @@
       <c r="E65" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="F65" s="15"/>
+      <c r="F65" s="13"/>
     </row>
     <row r="66" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="5" t="s">
@@ -2869,7 +2875,7 @@
         <v>19</v>
       </c>
       <c r="E66" s="7"/>
-      <c r="F66" s="15"/>
+      <c r="F66" s="13"/>
     </row>
     <row r="67" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="5" t="s">
@@ -2887,7 +2893,7 @@
       <c r="E67" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="F67" s="15"/>
+      <c r="F67" s="13"/>
     </row>
     <row r="68" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="5" t="s">
@@ -2905,7 +2911,7 @@
       <c r="E68" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="F68" s="15"/>
+      <c r="F68" s="13"/>
     </row>
     <row r="69" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="70" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2924,7 +2930,7 @@
       <c r="E70" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F70" s="15"/>
+      <c r="F70" s="13"/>
     </row>
     <row r="71" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
@@ -2940,7 +2946,7 @@
         <v>11</v>
       </c>
       <c r="E71" s="2"/>
-      <c r="F71" s="15"/>
+      <c r="F71" s="13"/>
     </row>
     <row r="72" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
@@ -2958,7 +2964,7 @@
       <c r="E72" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F72" s="15"/>
+      <c r="F72" s="13"/>
     </row>
     <row r="73" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="8" t="s">
@@ -2972,7 +2978,7 @@
       </c>
       <c r="D73" s="6"/>
       <c r="E73" s="7"/>
-      <c r="F73" s="15"/>
+      <c r="F73" s="13"/>
     </row>
     <row r="74" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="5" t="s">
@@ -2990,7 +2996,7 @@
       <c r="E74" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="F74" s="15"/>
+      <c r="F74" s="13"/>
     </row>
     <row r="75" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="5" t="s">
@@ -3008,7 +3014,7 @@
       <c r="E75" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="F75" s="15"/>
+      <c r="F75" s="13"/>
     </row>
     <row r="76" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="5" t="s">
@@ -3026,7 +3032,7 @@
       <c r="E76" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="F76" s="15"/>
+      <c r="F76" s="13"/>
     </row>
     <row r="77" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="78" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -3045,7 +3051,7 @@
       <c r="E78" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F78" s="15"/>
+      <c r="F78" s="13"/>
     </row>
     <row r="79" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
@@ -3061,7 +3067,7 @@
         <v>39</v>
       </c>
       <c r="E79" s="2"/>
-      <c r="F79" s="15"/>
+      <c r="F79" s="13"/>
     </row>
     <row r="80" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="3" t="s">
@@ -3079,7 +3085,7 @@
       <c r="E80" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F80" s="15"/>
+      <c r="F80" s="13"/>
     </row>
     <row r="81" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="8" t="s">
@@ -3093,7 +3099,7 @@
       </c>
       <c r="D81" s="6"/>
       <c r="E81" s="7"/>
-      <c r="F81" s="15"/>
+      <c r="F81" s="13"/>
     </row>
     <row r="82" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="5" t="s">
@@ -3111,7 +3117,7 @@
       <c r="E82" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="F82" s="15"/>
+      <c r="F82" s="13"/>
     </row>
     <row r="83" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="5" t="s">
@@ -3129,7 +3135,7 @@
       <c r="E83" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="F83" s="15"/>
+      <c r="F83" s="13"/>
     </row>
     <row r="84" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="5" t="s">
@@ -3147,7 +3153,7 @@
       <c r="E84" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="F84" s="15"/>
+      <c r="F84" s="13"/>
     </row>
     <row r="85" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="5" t="s">
@@ -3165,7 +3171,7 @@
       <c r="E85" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="F85" s="15"/>
+      <c r="F85" s="13"/>
     </row>
     <row r="86" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="5" t="s">
@@ -3183,7 +3189,7 @@
       <c r="E86" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="F86" s="15"/>
+      <c r="F86" s="13"/>
     </row>
     <row r="87" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="5" t="s">
@@ -3201,7 +3207,7 @@
       <c r="E87" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="F87" s="15"/>
+      <c r="F87" s="13"/>
     </row>
     <row r="88" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="89" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -3220,7 +3226,7 @@
       <c r="E89" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F89" s="15"/>
+      <c r="F89" s="13"/>
     </row>
     <row r="90" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="3" t="s">
@@ -3236,7 +3242,7 @@
         <v>11</v>
       </c>
       <c r="E90" s="2"/>
-      <c r="F90" s="15"/>
+      <c r="F90" s="13"/>
     </row>
     <row r="91" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="3" t="s">
@@ -3254,7 +3260,7 @@
       <c r="E91" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F91" s="15"/>
+      <c r="F91" s="13"/>
     </row>
     <row r="92" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="5" t="s">
@@ -3272,7 +3278,7 @@
       <c r="E92" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="F92" s="15"/>
+      <c r="F92" s="13"/>
     </row>
     <row r="93" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="94" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -3291,7 +3297,7 @@
       <c r="E94" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F94" s="15"/>
+      <c r="F94" s="13"/>
     </row>
     <row r="95" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="3" t="s">
@@ -3305,7 +3311,7 @@
         <v>39</v>
       </c>
       <c r="E95" s="2"/>
-      <c r="F95" s="15"/>
+      <c r="F95" s="13"/>
     </row>
     <row r="96" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="3" t="s">
@@ -3323,7 +3329,7 @@
       <c r="E96" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F96" s="15"/>
+      <c r="F96" s="13"/>
     </row>
     <row r="97" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="5" t="s">
@@ -3337,7 +3343,7 @@
       </c>
       <c r="D97" s="6"/>
       <c r="E97" s="7"/>
-      <c r="F97" s="15"/>
+      <c r="F97" s="13"/>
     </row>
     <row r="98" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="5" t="s">
@@ -3355,7 +3361,7 @@
       <c r="E98" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="F98" s="15"/>
+      <c r="F98" s="13"/>
     </row>
     <row r="99" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="100" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -3374,7 +3380,7 @@
       <c r="E100" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F100" s="15"/>
+      <c r="F100" s="13"/>
     </row>
     <row r="101" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="3" t="s">
@@ -3388,7 +3394,7 @@
         <v>39</v>
       </c>
       <c r="E101" s="2"/>
-      <c r="F101" s="15"/>
+      <c r="F101" s="13"/>
     </row>
     <row r="102" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="3" t="s">
@@ -3406,7 +3412,7 @@
       <c r="E102" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F102" s="15"/>
+      <c r="F102" s="13"/>
     </row>
     <row r="103" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="5" t="s">
@@ -3420,7 +3426,7 @@
       </c>
       <c r="D103" s="6"/>
       <c r="E103" s="7"/>
-      <c r="F103" s="15"/>
+      <c r="F103" s="13"/>
     </row>
     <row r="104" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="5" t="s">
@@ -3438,7 +3444,7 @@
       <c r="E104" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="F104" s="15"/>
+      <c r="F104" s="13"/>
     </row>
     <row r="105" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="106" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -3457,7 +3463,7 @@
       <c r="E106" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F106" s="15"/>
+      <c r="F106" s="13"/>
     </row>
     <row r="107" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="3" t="s">
@@ -3471,7 +3477,7 @@
         <v>19</v>
       </c>
       <c r="E107" s="2"/>
-      <c r="F107" s="15"/>
+      <c r="F107" s="13"/>
     </row>
     <row r="108" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="3" t="s">
@@ -3489,7 +3495,7 @@
       <c r="E108" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F108" s="15"/>
+      <c r="F108" s="13"/>
     </row>
     <row r="109" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="5" t="s">
@@ -3507,7 +3513,7 @@
       <c r="E109" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="F109" s="15"/>
+      <c r="F109" s="13"/>
     </row>
     <row r="110" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="5" t="s">
@@ -3525,7 +3531,7 @@
       <c r="E110" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="F110" s="15"/>
+      <c r="F110" s="13"/>
     </row>
     <row r="111" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="5" t="s">
@@ -3543,7 +3549,7 @@
       <c r="E111" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="F111" s="15"/>
+      <c r="F111" s="13"/>
     </row>
     <row r="112" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="5" t="s">
@@ -3561,7 +3567,7 @@
       <c r="E112" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="F112" s="15"/>
+      <c r="F112" s="13"/>
     </row>
     <row r="113" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="5" t="s">
@@ -3579,7 +3585,7 @@
       <c r="E113" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="F113" s="15"/>
+      <c r="F113" s="13"/>
     </row>
     <row r="114" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="5" t="s">
@@ -3597,7 +3603,7 @@
       <c r="E114" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="F114" s="15"/>
+      <c r="F114" s="13"/>
     </row>
     <row r="115" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="5" t="s">
@@ -3615,7 +3621,7 @@
       <c r="E115" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="F115" s="15"/>
+      <c r="F115" s="13"/>
     </row>
     <row r="116" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="5" t="s">
@@ -3633,7 +3639,7 @@
       <c r="E116" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="F116" s="15"/>
+      <c r="F116" s="13"/>
     </row>
     <row r="117" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="118" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -3652,7 +3658,7 @@
       <c r="E118" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F118" s="15"/>
+      <c r="F118" s="13"/>
     </row>
     <row r="119" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="3" t="s">
@@ -3666,7 +3672,7 @@
         <v>19</v>
       </c>
       <c r="E119" s="2"/>
-      <c r="F119" s="15"/>
+      <c r="F119" s="13"/>
     </row>
     <row r="120" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="3" t="s">
@@ -3684,7 +3690,7 @@
       <c r="E120" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F120" s="15"/>
+      <c r="F120" s="13"/>
     </row>
     <row r="121" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="5" t="s">
@@ -3702,7 +3708,7 @@
       <c r="E121" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="F121" s="15"/>
+      <c r="F121" s="13"/>
     </row>
     <row r="122" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="5" t="s">
@@ -3720,7 +3726,7 @@
       <c r="E122" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="F122" s="15"/>
+      <c r="F122" s="13"/>
     </row>
     <row r="123" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="5" t="s">
@@ -3738,7 +3744,7 @@
       <c r="E123" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="F123" s="15"/>
+      <c r="F123" s="13"/>
     </row>
     <row r="124" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="125" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -3757,7 +3763,7 @@
       <c r="E125" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F125" s="15"/>
+      <c r="F125" s="13"/>
     </row>
     <row r="126" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="3" t="s">
@@ -3771,7 +3777,7 @@
         <v>39</v>
       </c>
       <c r="E126" s="2"/>
-      <c r="F126" s="15"/>
+      <c r="F126" s="13"/>
     </row>
     <row r="127" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="3" t="s">
@@ -3789,7 +3795,7 @@
       <c r="E127" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F127" s="15"/>
+      <c r="F127" s="13"/>
     </row>
     <row r="128" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="5" t="s">
@@ -3803,9 +3809,9 @@
       </c>
       <c r="D128" s="6"/>
       <c r="E128" s="7"/>
-      <c r="F128" s="15"/>
-    </row>
-    <row r="129" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F128" s="13"/>
+    </row>
+    <row r="129" spans="1:7" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="5" t="s">
         <v>213</v>
       </c>
@@ -3813,9 +3819,9 @@
       <c r="C129" s="2"/>
       <c r="D129" s="2"/>
       <c r="E129" s="2"/>
-      <c r="F129" s="15"/>
-    </row>
-    <row r="130" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F129" s="13"/>
+    </row>
+    <row r="130" spans="1:7" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="5" t="s">
         <v>214</v>
       </c>
@@ -3831,9 +3837,9 @@
       <c r="E130" s="7" t="s">
         <v>216</v>
       </c>
-      <c r="F130" s="15"/>
-    </row>
-    <row r="131" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F130" s="13"/>
+    </row>
+    <row r="131" spans="1:7" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="5" t="s">
         <v>217</v>
       </c>
@@ -3849,9 +3855,9 @@
       <c r="E131" s="7" t="s">
         <v>219</v>
       </c>
-      <c r="F131" s="15"/>
-    </row>
-    <row r="132" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F131" s="13"/>
+    </row>
+    <row r="132" spans="1:7" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="5" t="s">
         <v>220</v>
       </c>
@@ -3867,9 +3873,9 @@
       <c r="E132" s="7" t="s">
         <v>222</v>
       </c>
-      <c r="F132" s="15"/>
-    </row>
-    <row r="133" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F132" s="13"/>
+    </row>
+    <row r="133" spans="1:7" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="5" t="s">
         <v>223</v>
       </c>
@@ -3885,9 +3891,9 @@
       <c r="E133" s="7" t="s">
         <v>225</v>
       </c>
-      <c r="F133" s="15"/>
-    </row>
-    <row r="134" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F133" s="13"/>
+    </row>
+    <row r="134" spans="1:7" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="5" t="s">
         <v>226</v>
       </c>
@@ -3903,9 +3909,9 @@
       <c r="E134" s="7" t="s">
         <v>228</v>
       </c>
-      <c r="F134" s="15"/>
-    </row>
-    <row r="135" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F134" s="13"/>
+    </row>
+    <row r="135" spans="1:7" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="5" t="s">
         <v>229</v>
       </c>
@@ -3921,9 +3927,9 @@
       <c r="E135" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="F135" s="15"/>
-    </row>
-    <row r="136" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F135" s="13"/>
+    </row>
+    <row r="136" spans="1:7" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" s="5" t="s">
         <v>231</v>
       </c>
@@ -3939,9 +3945,9 @@
       <c r="E136" s="7" t="s">
         <v>233</v>
       </c>
-      <c r="F136" s="15"/>
-    </row>
-    <row r="137" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F136" s="13"/>
+    </row>
+    <row r="137" spans="1:7" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="5" t="s">
         <v>234</v>
       </c>
@@ -3957,9 +3963,9 @@
       <c r="E137" s="7" t="s">
         <v>233</v>
       </c>
-      <c r="F137" s="15"/>
-    </row>
-    <row r="138" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F137" s="13"/>
+    </row>
+    <row r="138" spans="1:7" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A138" s="5" t="s">
         <v>236</v>
       </c>
@@ -3975,13 +3981,15 @@
       <c r="E138" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="F138" s="15"/>
-    </row>
-    <row r="139" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F138" s="13"/>
+    </row>
+    <row r="139" spans="1:7" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139" s="5" t="s">
         <v>238</v>
       </c>
-      <c r="B139" s="6"/>
+      <c r="B139" s="8" t="s">
+        <v>408</v>
+      </c>
       <c r="C139" s="6" t="s">
         <v>32</v>
       </c>
@@ -3991,9 +3999,12 @@
       <c r="E139" s="7" t="s">
         <v>239</v>
       </c>
-      <c r="F139" s="15"/>
-    </row>
-    <row r="140" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F139" s="13"/>
+      <c r="G139" s="12" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" s="5" t="s">
         <v>240</v>
       </c>
@@ -4009,11 +4020,11 @@
       <c r="E140" s="7" t="s">
         <v>242</v>
       </c>
-      <c r="F140" s="17" t="s">
+      <c r="F140" s="15" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="141" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:7" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141" s="5" t="s">
         <v>244</v>
       </c>
@@ -4029,11 +4040,11 @@
       <c r="E141" s="7" t="s">
         <v>246</v>
       </c>
-      <c r="F141" s="17" t="s">
+      <c r="F141" s="15" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="142" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:7" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A142" s="5" t="s">
         <v>247</v>
       </c>
@@ -4049,9 +4060,9 @@
       <c r="E142" s="7" t="s">
         <v>249</v>
       </c>
-      <c r="F142" s="15"/>
-    </row>
-    <row r="143" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F142" s="13"/>
+    </row>
+    <row r="143" spans="1:7" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A143" s="5" t="s">
         <v>250</v>
       </c>
@@ -4067,9 +4078,9 @@
       <c r="E143" s="7" t="s">
         <v>252</v>
       </c>
-      <c r="F143" s="15"/>
-    </row>
-    <row r="144" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F143" s="13"/>
+    </row>
+    <row r="144" spans="1:7" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A144" s="5" t="s">
         <v>254</v>
       </c>
@@ -4083,7 +4094,7 @@
         <v>39</v>
       </c>
       <c r="E144" s="7"/>
-      <c r="F144" s="17" t="s">
+      <c r="F144" s="15" t="s">
         <v>243</v>
       </c>
     </row>
@@ -4103,7 +4114,7 @@
       <c r="E145" s="7" t="s">
         <v>258</v>
       </c>
-      <c r="F145" s="17" t="s">
+      <c r="F145" s="15" t="s">
         <v>243</v>
       </c>
     </row>
@@ -4123,7 +4134,7 @@
       <c r="E146" s="7" t="s">
         <v>261</v>
       </c>
-      <c r="F146" s="17" t="s">
+      <c r="F146" s="15" t="s">
         <v>243</v>
       </c>
     </row>
@@ -4143,7 +4154,7 @@
       <c r="E147" s="7" t="s">
         <v>261</v>
       </c>
-      <c r="F147" s="17" t="s">
+      <c r="F147" s="15" t="s">
         <v>243</v>
       </c>
     </row>
@@ -4163,7 +4174,7 @@
       <c r="E148" s="7" t="s">
         <v>266</v>
       </c>
-      <c r="F148" s="17" t="s">
+      <c r="F148" s="15" t="s">
         <v>243</v>
       </c>
     </row>
@@ -4183,7 +4194,7 @@
       <c r="E149" s="7" t="s">
         <v>269</v>
       </c>
-      <c r="F149" s="17" t="s">
+      <c r="F149" s="15" t="s">
         <v>243</v>
       </c>
     </row>
@@ -4203,7 +4214,7 @@
       <c r="E150" s="7" t="s">
         <v>272</v>
       </c>
-      <c r="F150" s="17" t="s">
+      <c r="F150" s="15" t="s">
         <v>243</v>
       </c>
     </row>
@@ -4215,7 +4226,7 @@
       <c r="C151" s="6"/>
       <c r="D151" s="6"/>
       <c r="E151" s="7"/>
-      <c r="F151" s="17" t="s">
+      <c r="F151" s="15" t="s">
         <v>243</v>
       </c>
     </row>
@@ -4233,7 +4244,7 @@
         <v>39</v>
       </c>
       <c r="E152" s="7"/>
-      <c r="F152" s="15"/>
+      <c r="F152" s="13"/>
     </row>
     <row r="153" spans="1:7" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A153" s="5" t="s">
@@ -4251,7 +4262,7 @@
       <c r="E153" s="7" t="s">
         <v>278</v>
       </c>
-      <c r="F153" s="15"/>
+      <c r="F153" s="13"/>
     </row>
     <row r="154" spans="1:7" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A154" s="5" t="s">
@@ -4269,7 +4280,7 @@
       <c r="E154" s="7" t="s">
         <v>280</v>
       </c>
-      <c r="F154" s="15"/>
+      <c r="F154" s="13"/>
     </row>
     <row r="155" spans="1:7" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A155" s="5" t="s">
@@ -4287,7 +4298,7 @@
       <c r="E155" s="7" t="s">
         <v>283</v>
       </c>
-      <c r="F155" s="15"/>
+      <c r="F155" s="13"/>
     </row>
     <row r="156" spans="1:7" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A156" s="5" t="s">
@@ -4305,7 +4316,7 @@
       <c r="E156" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="F156" s="15"/>
+      <c r="F156" s="13"/>
     </row>
     <row r="157" spans="1:7" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A157" s="5" t="s">
@@ -4323,7 +4334,7 @@
       <c r="E157" s="7" t="s">
         <v>288</v>
       </c>
-      <c r="F157" s="17" t="s">
+      <c r="F157" s="15" t="s">
         <v>243</v>
       </c>
     </row>
@@ -4335,7 +4346,7 @@
       <c r="C158" s="6"/>
       <c r="D158" s="6"/>
       <c r="E158" s="7"/>
-      <c r="F158" s="17"/>
+      <c r="F158" s="15"/>
     </row>
     <row r="159" spans="1:7" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A159" s="8" t="s">
@@ -4345,7 +4356,7 @@
       <c r="C159" s="6"/>
       <c r="D159" s="6"/>
       <c r="E159" s="7"/>
-      <c r="F159" s="15"/>
+      <c r="F159" s="13"/>
       <c r="G159" s="12" t="s">
         <v>404</v>
       </c>
@@ -4366,7 +4377,7 @@
       <c r="E160" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="F160" s="15"/>
+      <c r="F160" s="13"/>
       <c r="G160" s="12" t="s">
         <v>403</v>
       </c>
@@ -4383,7 +4394,7 @@
       </c>
       <c r="D161" s="6"/>
       <c r="E161" s="7"/>
-      <c r="F161" s="15"/>
+      <c r="F161" s="13"/>
       <c r="G161" s="12" t="s">
         <v>407</v>
       </c>
@@ -4392,11 +4403,11 @@
       <c r="A162" s="8" t="s">
         <v>406</v>
       </c>
-      <c r="B162" s="18"/>
-      <c r="C162" s="18"/>
-      <c r="D162" s="18"/>
-      <c r="E162" s="19"/>
-      <c r="F162" s="15"/>
+      <c r="B162" s="16"/>
+      <c r="C162" s="16"/>
+      <c r="D162" s="16"/>
+      <c r="E162" s="17"/>
+      <c r="F162" s="13"/>
     </row>
     <row r="163" spans="1:7" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A163" s="5" t="s">
@@ -4414,7 +4425,7 @@
       <c r="E163" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="F163" s="15"/>
+      <c r="F163" s="13"/>
     </row>
     <row r="164" spans="1:7" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A164" s="5" t="s">
@@ -4432,7 +4443,7 @@
       <c r="E164" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="F164" s="15"/>
+      <c r="F164" s="13"/>
     </row>
     <row r="165" spans="1:7" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A165" s="5" t="s">
@@ -4450,7 +4461,7 @@
       <c r="E165" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="F165" s="15"/>
+      <c r="F165" s="13"/>
     </row>
     <row r="166" spans="1:7" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A166" s="5" t="s">
@@ -4468,7 +4479,7 @@
       <c r="E166" s="7" t="s">
         <v>283</v>
       </c>
-      <c r="F166" s="15"/>
+      <c r="F166" s="13"/>
     </row>
     <row r="167" spans="1:7" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A167" s="5" t="s">
@@ -4486,7 +4497,7 @@
       <c r="E167" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="F167" s="15"/>
+      <c r="F167" s="13"/>
     </row>
     <row r="168" spans="1:7" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A168" s="5" t="s">
@@ -4504,7 +4515,7 @@
       <c r="E168" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="F168" s="15"/>
+      <c r="F168" s="13"/>
     </row>
     <row r="169" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="170" spans="1:7" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -4523,7 +4534,7 @@
       <c r="E170" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F170" s="15"/>
+      <c r="F170" s="13"/>
     </row>
     <row r="171" spans="1:7" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A171" s="3" t="s">
@@ -4539,7 +4550,7 @@
         <v>11</v>
       </c>
       <c r="E171" s="2"/>
-      <c r="F171" s="15"/>
+      <c r="F171" s="13"/>
     </row>
     <row r="172" spans="1:7" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A172" s="3" t="s">
@@ -4557,7 +4568,7 @@
       <c r="E172" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F172" s="15"/>
+      <c r="F172" s="13"/>
     </row>
     <row r="173" spans="1:7" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A173" s="9" t="s">
@@ -4571,7 +4582,7 @@
       </c>
       <c r="D173" s="6"/>
       <c r="E173" s="7"/>
-      <c r="F173" s="15"/>
+      <c r="F173" s="13"/>
     </row>
     <row r="174" spans="1:7" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A174" s="5" t="s">
@@ -4589,7 +4600,7 @@
       <c r="E174" s="7" t="s">
         <v>307</v>
       </c>
-      <c r="F174" s="15"/>
+      <c r="F174" s="13"/>
     </row>
     <row r="175" spans="1:7" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A175" s="5" t="s">
@@ -4599,7 +4610,7 @@
       <c r="C175" s="6"/>
       <c r="D175" s="6"/>
       <c r="E175" s="7"/>
-      <c r="F175" s="15"/>
+      <c r="F175" s="13"/>
     </row>
     <row r="176" spans="1:7" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A176" s="5" t="s">
@@ -4617,7 +4628,7 @@
       <c r="E176" s="7" t="s">
         <v>311</v>
       </c>
-      <c r="F176" s="15"/>
+      <c r="F176" s="13"/>
     </row>
     <row r="177" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A177" s="5" t="s">
@@ -4635,7 +4646,7 @@
       <c r="E177" s="7" t="s">
         <v>314</v>
       </c>
-      <c r="F177" s="15"/>
+      <c r="F177" s="13"/>
     </row>
     <row r="178" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A178" s="5" t="s">
@@ -4653,7 +4664,7 @@
       <c r="E178" s="7" t="s">
         <v>317</v>
       </c>
-      <c r="F178" s="15"/>
+      <c r="F178" s="13"/>
     </row>
     <row r="179" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A179" s="5" t="s">
@@ -4671,7 +4682,7 @@
       <c r="E179" s="7" t="s">
         <v>320</v>
       </c>
-      <c r="F179" s="15"/>
+      <c r="F179" s="13"/>
     </row>
     <row r="180" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A180" s="5" t="s">
@@ -4689,7 +4700,7 @@
       <c r="E180" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="F180" s="15"/>
+      <c r="F180" s="13"/>
     </row>
     <row r="181" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A181" s="9" t="s">
@@ -4699,7 +4710,7 @@
       <c r="C181" s="10"/>
       <c r="D181" s="10"/>
       <c r="E181" s="11"/>
-      <c r="F181" s="15"/>
+      <c r="F181" s="13"/>
     </row>
     <row r="182" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A182" s="5" t="s">
@@ -4717,7 +4728,7 @@
       <c r="E182" s="7" t="s">
         <v>325</v>
       </c>
-      <c r="F182" s="15"/>
+      <c r="F182" s="13"/>
     </row>
     <row r="183" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A183" s="5" t="s">
@@ -4735,7 +4746,7 @@
       <c r="E183" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="F183" s="15"/>
+      <c r="F183" s="13"/>
     </row>
     <row r="184" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A184" s="5" t="s">
@@ -4753,7 +4764,7 @@
       <c r="E184" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="F184" s="15"/>
+      <c r="F184" s="13"/>
     </row>
     <row r="185" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="186" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -4772,7 +4783,7 @@
       <c r="E186" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F186" s="15"/>
+      <c r="F186" s="13"/>
     </row>
     <row r="187" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A187" s="3" t="s">
@@ -4786,7 +4797,7 @@
         <v>19</v>
       </c>
       <c r="E187" s="2"/>
-      <c r="F187" s="15"/>
+      <c r="F187" s="13"/>
     </row>
     <row r="188" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A188" s="3" t="s">
@@ -4804,7 +4815,7 @@
       <c r="E188" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F188" s="15"/>
+      <c r="F188" s="13"/>
     </row>
     <row r="189" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A189" s="5" t="s">
@@ -4822,7 +4833,7 @@
       <c r="E189" s="7" t="s">
         <v>333</v>
       </c>
-      <c r="F189" s="15"/>
+      <c r="F189" s="13"/>
     </row>
     <row r="190" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A190" s="5" t="s">
@@ -4840,7 +4851,7 @@
       <c r="E190" s="7" t="s">
         <v>336</v>
       </c>
-      <c r="F190" s="15"/>
+      <c r="F190" s="13"/>
     </row>
     <row r="191" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="192" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -4859,7 +4870,7 @@
       <c r="E192" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F192" s="15"/>
+      <c r="F192" s="13"/>
     </row>
     <row r="193" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A193" s="3" t="s">
@@ -4873,7 +4884,7 @@
         <v>19</v>
       </c>
       <c r="E193" s="2"/>
-      <c r="F193" s="15"/>
+      <c r="F193" s="13"/>
     </row>
     <row r="194" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A194" s="3" t="s">
@@ -4891,7 +4902,7 @@
       <c r="E194" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F194" s="15"/>
+      <c r="F194" s="13"/>
     </row>
     <row r="195" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A195" s="5" t="s">
@@ -4909,7 +4920,7 @@
       <c r="E195" s="7" t="s">
         <v>340</v>
       </c>
-      <c r="F195" s="15"/>
+      <c r="F195" s="13"/>
     </row>
     <row r="196" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="197" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -4928,7 +4939,7 @@
       <c r="E197" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F197" s="15"/>
+      <c r="F197" s="13"/>
     </row>
     <row r="198" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A198" s="3" t="s">
@@ -4942,7 +4953,7 @@
         <v>19</v>
       </c>
       <c r="E198" s="2"/>
-      <c r="F198" s="15"/>
+      <c r="F198" s="13"/>
     </row>
     <row r="199" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A199" s="3" t="s">
@@ -4960,7 +4971,7 @@
       <c r="E199" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F199" s="15"/>
+      <c r="F199" s="13"/>
     </row>
     <row r="200" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A200" s="5" t="s">
@@ -4974,7 +4985,7 @@
       </c>
       <c r="D200" s="6"/>
       <c r="E200" s="7"/>
-      <c r="F200" s="15" t="s">
+      <c r="F200" s="13" t="s">
         <v>243</v>
       </c>
     </row>
@@ -4994,7 +5005,7 @@
       <c r="E201" s="7" t="s">
         <v>346</v>
       </c>
-      <c r="F201" s="15"/>
+      <c r="F201" s="13"/>
     </row>
     <row r="202" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A202" s="5" t="s">
@@ -5012,7 +5023,7 @@
       <c r="E202" s="7" t="s">
         <v>349</v>
       </c>
-      <c r="F202" s="15"/>
+      <c r="F202" s="13"/>
     </row>
     <row r="203" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A203" s="5" t="s">
@@ -5030,7 +5041,7 @@
       <c r="E203" s="7" t="s">
         <v>352</v>
       </c>
-      <c r="F203" s="15"/>
+      <c r="F203" s="13"/>
     </row>
     <row r="204" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A204" s="5" t="s">
@@ -5048,7 +5059,7 @@
       <c r="E204" s="7" t="s">
         <v>355</v>
       </c>
-      <c r="F204" s="15"/>
+      <c r="F204" s="13"/>
     </row>
     <row r="205" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A205" s="5" t="s">
@@ -5066,7 +5077,7 @@
       <c r="E205" s="7" t="s">
         <v>358</v>
       </c>
-      <c r="F205" s="15"/>
+      <c r="F205" s="13"/>
     </row>
     <row r="206" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="207" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -5085,7 +5096,7 @@
       <c r="E207" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F207" s="15"/>
+      <c r="F207" s="13"/>
     </row>
     <row r="208" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A208" s="3" t="s">
@@ -5101,7 +5112,7 @@
         <v>11</v>
       </c>
       <c r="E208" s="2"/>
-      <c r="F208" s="15"/>
+      <c r="F208" s="13"/>
     </row>
     <row r="209" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A209" s="3" t="s">
@@ -5119,7 +5130,7 @@
       <c r="E209" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F209" s="15"/>
+      <c r="F209" s="13"/>
     </row>
     <row r="210" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A210" s="5" t="s">
@@ -5137,7 +5148,7 @@
       <c r="E210" s="7" t="s">
         <v>363</v>
       </c>
-      <c r="F210" s="15"/>
+      <c r="F210" s="13"/>
     </row>
     <row r="211" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A211" s="5" t="s">
@@ -5155,7 +5166,7 @@
       <c r="E211" s="7" t="s">
         <v>366</v>
       </c>
-      <c r="F211" s="15"/>
+      <c r="F211" s="13"/>
     </row>
     <row r="212" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A212" s="5" t="s">
@@ -5173,7 +5184,7 @@
       <c r="E212" s="7" t="s">
         <v>369</v>
       </c>
-      <c r="F212" s="15"/>
+      <c r="F212" s="13"/>
     </row>
     <row r="213" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A213" s="5" t="s">
@@ -5191,7 +5202,7 @@
       <c r="E213" s="7" t="s">
         <v>372</v>
       </c>
-      <c r="F213" s="15"/>
+      <c r="F213" s="13"/>
     </row>
     <row r="214" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A214" s="5" t="s">
@@ -5209,7 +5220,7 @@
       <c r="E214" s="7" t="s">
         <v>375</v>
       </c>
-      <c r="F214" s="15"/>
+      <c r="F214" s="13"/>
     </row>
     <row r="215" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A215" s="5" t="s">
@@ -5227,7 +5238,7 @@
       <c r="E215" s="7" t="s">
         <v>378</v>
       </c>
-      <c r="F215" s="15"/>
+      <c r="F215" s="13"/>
     </row>
     <row r="216" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A216" s="5" t="s">
@@ -5245,7 +5256,7 @@
       <c r="E216" s="7" t="s">
         <v>381</v>
       </c>
-      <c r="F216" s="15"/>
+      <c r="F216" s="13"/>
     </row>
     <row r="217" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A217" s="5" t="s">
@@ -5263,7 +5274,7 @@
       <c r="E217" s="7" t="s">
         <v>384</v>
       </c>
-      <c r="F217" s="15"/>
+      <c r="F217" s="13"/>
     </row>
     <row r="218" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="219" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -5282,7 +5293,7 @@
       <c r="E219" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F219" s="15"/>
+      <c r="F219" s="13"/>
     </row>
     <row r="220" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A220" s="3" t="s">
@@ -5296,7 +5307,7 @@
         <v>19</v>
       </c>
       <c r="E220" s="2"/>
-      <c r="F220" s="15"/>
+      <c r="F220" s="13"/>
     </row>
     <row r="221" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A221" s="3" t="s">
@@ -5314,7 +5325,7 @@
       <c r="E221" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F221" s="15"/>
+      <c r="F221" s="13"/>
     </row>
     <row r="222" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A222" s="5" t="s">
@@ -5328,7 +5339,7 @@
       </c>
       <c r="D222" s="6"/>
       <c r="E222" s="7"/>
-      <c r="F222" s="15"/>
+      <c r="F222" s="13"/>
     </row>
     <row r="223" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A223" s="5" t="s">
@@ -5346,7 +5357,7 @@
       <c r="E223" s="7" t="s">
         <v>389</v>
       </c>
-      <c r="F223" s="15"/>
+      <c r="F223" s="13"/>
     </row>
     <row r="224" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A224" s="5" t="s">
@@ -5364,7 +5375,7 @@
       <c r="E224" s="7" t="s">
         <v>391</v>
       </c>
-      <c r="F224" s="15"/>
+      <c r="F224" s="13"/>
     </row>
     <row r="225" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A225" s="5" t="s">
@@ -5382,7 +5393,7 @@
       <c r="E225" s="7" t="s">
         <v>393</v>
       </c>
-      <c r="F225" s="15"/>
+      <c r="F225" s="13"/>
     </row>
     <row r="226" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A226" s="5" t="s">
@@ -5400,7 +5411,7 @@
       <c r="E226" s="7" t="s">
         <v>396</v>
       </c>
-      <c r="F226" s="15"/>
+      <c r="F226" s="13"/>
     </row>
     <row r="227" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A227" s="5" t="s">
@@ -5418,7 +5429,7 @@
       <c r="E227" s="7" t="s">
         <v>399</v>
       </c>
-      <c r="F227" s="15"/>
+      <c r="F227" s="13"/>
     </row>
     <row r="228" spans="1:6" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A228" s="5" t="s">
@@ -5436,7 +5447,7 @@
       <c r="E228" s="7" t="s">
         <v>402</v>
       </c>
-      <c r="F228" s="15"/>
+      <c r="F228" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Move item cluster to original position
</commit_message>
<xml_diff>
--- a/guidelines/eDischarge-Summary-v2.1-1st-Feb-21.xlsx
+++ b/guidelines/eDischarge-Summary-v2.1-1st-Feb-21.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/simonellershaw/Documents/discharge-summaries/guidelines/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B347C508-13DE-9E49-98C8-77AE0C22C4AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD5E2146-FABC-F042-BB9D-B3EA47CFA5C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="947" uniqueCount="410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="946" uniqueCount="409">
   <si>
     <t>E Discharge</t>
   </si>
@@ -1294,9 +1294,6 @@
   </si>
   <si>
     <t>Remove repeated entry</t>
-  </si>
-  <si>
-    <t>The position of this cluster end is different to that of FHIR but makes greater semantic sense</t>
   </si>
   <si>
     <r>
@@ -1338,7 +1335,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1393,6 +1390,11 @@
       <b/>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri (Body)"/>
     </font>
   </fonts>
@@ -1495,7 +1497,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1553,6 +1555,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1861,8 +1869,8 @@
   </sheetPr>
   <dimension ref="A1:G228"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
-      <selection activeCell="G134" sqref="G134"/>
+    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
+      <selection activeCell="A144" sqref="A144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3988,7 +3996,7 @@
         <v>238</v>
       </c>
       <c r="B139" s="8" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C139" s="6" t="s">
         <v>32</v>
@@ -4001,7 +4009,7 @@
       </c>
       <c r="F139" s="13"/>
       <c r="G139" s="12" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="140" spans="1:7" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -4080,30 +4088,22 @@
       </c>
       <c r="F143" s="13"/>
     </row>
-    <row r="144" spans="1:7" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A144" s="5" t="s">
-        <v>254</v>
-      </c>
-      <c r="B144" s="6" t="s">
-        <v>255</v>
-      </c>
-      <c r="C144" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D144" s="6" t="s">
-        <v>39</v>
-      </c>
+    <row r="144" spans="1:7" s="21" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A144" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="B144" s="6"/>
+      <c r="C144" s="6"/>
+      <c r="D144" s="6"/>
       <c r="E144" s="7"/>
-      <c r="F144" s="15" t="s">
-        <v>243</v>
-      </c>
+      <c r="F144" s="20"/>
     </row>
     <row r="145" spans="1:7" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A145" s="5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B145" s="6" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C145" s="6" t="s">
         <v>18</v>
@@ -4111,19 +4111,17 @@
       <c r="D145" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="E145" s="7" t="s">
-        <v>258</v>
-      </c>
+      <c r="E145" s="7"/>
       <c r="F145" s="15" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="146" spans="1:7" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A146" s="5" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B146" s="6" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C146" s="6" t="s">
         <v>18</v>
@@ -4132,7 +4130,7 @@
         <v>39</v>
       </c>
       <c r="E146" s="7" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="F146" s="15" t="s">
         <v>243</v>
@@ -4140,10 +4138,10 @@
     </row>
     <row r="147" spans="1:7" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A147" s="5" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="B147" s="6" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C147" s="6" t="s">
         <v>18</v>
@@ -4160,10 +4158,10 @@
     </row>
     <row r="148" spans="1:7" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A148" s="5" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B148" s="6" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C148" s="6" t="s">
         <v>18</v>
@@ -4172,7 +4170,7 @@
         <v>39</v>
       </c>
       <c r="E148" s="7" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="F148" s="15" t="s">
         <v>243</v>
@@ -4180,10 +4178,10 @@
     </row>
     <row r="149" spans="1:7" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A149" s="5" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="B149" s="6" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="C149" s="6" t="s">
         <v>18</v>
@@ -4192,7 +4190,7 @@
         <v>39</v>
       </c>
       <c r="E149" s="7" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F149" s="15" t="s">
         <v>243</v>
@@ -4200,10 +4198,10 @@
     </row>
     <row r="150" spans="1:7" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A150" s="5" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="B150" s="6" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="C150" s="6" t="s">
         <v>18</v>
@@ -4212,46 +4210,50 @@
         <v>39</v>
       </c>
       <c r="E150" s="7" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F150" s="15" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="151" spans="1:7" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A151" s="8" t="s">
-        <v>273</v>
-      </c>
-      <c r="B151" s="6"/>
-      <c r="C151" s="6"/>
-      <c r="D151" s="6"/>
-      <c r="E151" s="7"/>
+      <c r="A151" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="B151" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="C151" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D151" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E151" s="7" t="s">
+        <v>272</v>
+      </c>
       <c r="F151" s="15" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="152" spans="1:7" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A152" s="5" t="s">
-        <v>274</v>
-      </c>
-      <c r="B152" s="6" t="s">
-        <v>275</v>
-      </c>
-      <c r="C152" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D152" s="6" t="s">
-        <v>39</v>
-      </c>
+      <c r="A152" s="8" t="s">
+        <v>273</v>
+      </c>
+      <c r="B152" s="6"/>
+      <c r="C152" s="6"/>
+      <c r="D152" s="6"/>
       <c r="E152" s="7"/>
-      <c r="F152" s="13"/>
+      <c r="F152" s="15" t="s">
+        <v>243</v>
+      </c>
     </row>
     <row r="153" spans="1:7" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A153" s="5" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B153" s="6" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C153" s="6" t="s">
         <v>18</v>
@@ -4259,17 +4261,15 @@
       <c r="D153" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="E153" s="7" t="s">
-        <v>278</v>
-      </c>
+      <c r="E153" s="7"/>
       <c r="F153" s="13"/>
     </row>
     <row r="154" spans="1:7" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A154" s="5" t="s">
-        <v>264</v>
+        <v>276</v>
       </c>
       <c r="B154" s="6" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C154" s="6" t="s">
         <v>18</v>
@@ -4278,16 +4278,16 @@
         <v>39</v>
       </c>
       <c r="E154" s="7" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="F154" s="13"/>
     </row>
     <row r="155" spans="1:7" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A155" s="5" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="B155" s="6" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="C155" s="6" t="s">
         <v>18</v>
@@ -4296,16 +4296,16 @@
         <v>39</v>
       </c>
       <c r="E155" s="7" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="F155" s="13"/>
     </row>
     <row r="156" spans="1:7" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A156" s="5" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="B156" s="6" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="C156" s="6" t="s">
         <v>18</v>
@@ -4314,52 +4314,57 @@
         <v>39</v>
       </c>
       <c r="E156" s="7" t="s">
-        <v>157</v>
+        <v>283</v>
       </c>
       <c r="F156" s="13"/>
     </row>
     <row r="157" spans="1:7" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A157" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="B157" s="6" t="s">
+        <v>285</v>
+      </c>
+      <c r="C157" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D157" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E157" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="F157" s="13"/>
+    </row>
+    <row r="158" spans="1:7" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A158" s="5" t="s">
         <v>286</v>
       </c>
-      <c r="B157" s="6" t="s">
+      <c r="B158" s="6" t="s">
         <v>287</v>
       </c>
-      <c r="C157" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D157" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E157" s="7" t="s">
+      <c r="C158" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D158" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E158" s="7" t="s">
         <v>288</v>
       </c>
-      <c r="F157" s="15" t="s">
+      <c r="F158" s="15" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="158" spans="1:7" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A158" s="8" t="s">
-        <v>289</v>
-      </c>
-      <c r="B158" s="6"/>
-      <c r="C158" s="6"/>
-      <c r="D158" s="6"/>
-      <c r="E158" s="7"/>
-      <c r="F158" s="15"/>
     </row>
     <row r="159" spans="1:7" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A159" s="8" t="s">
-        <v>253</v>
+        <v>289</v>
       </c>
       <c r="B159" s="6"/>
       <c r="C159" s="6"/>
       <c r="D159" s="6"/>
       <c r="E159" s="7"/>
-      <c r="F159" s="13"/>
-      <c r="G159" s="12" t="s">
-        <v>404</v>
-      </c>
+      <c r="F159" s="15"/>
     </row>
     <row r="160" spans="1:7" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A160" s="5" t="s">
@@ -4384,7 +4389,7 @@
     </row>
     <row r="161" spans="1:7" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A161" s="5" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B161" s="6" t="s">
         <v>292</v>
@@ -4396,12 +4401,12 @@
       <c r="E161" s="7"/>
       <c r="F161" s="13"/>
       <c r="G161" s="12" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="162" spans="1:7" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A162" s="8" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B162" s="16"/>
       <c r="C162" s="16"/>

</xml_diff>